<commit_message>
ajout patients, spécialité, IHM, update recherche
</commit_message>
<xml_diff>
--- a/server/delire/data.xlsx
+++ b/server/delire/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\pomme\server\delire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathilde/Documents/pomme/server/delire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20AF3D-5D84-42A7-A5EA-07CBC7F3DA2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="8145" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PersonneClient" sheetId="1" r:id="rId1"/>
@@ -22,16 +21,16 @@
     <sheet name="EmpSpe" sheetId="7" r:id="rId7"/>
     <sheet name="NoeudSpe" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="193">
   <si>
     <t>var</t>
   </si>
@@ -94,9 +93,6 @@
     <t>01.01.01.01.01</t>
   </si>
   <si>
-    <t>10 rue de la rue, 75001, Paris</t>
-  </si>
-  <si>
     <t>PC2</t>
   </si>
   <si>
@@ -112,9 +108,6 @@
     <t>02.02.02.02.02</t>
   </si>
   <si>
-    <t>20 allée de l'allée, 75002, Paris</t>
-  </si>
-  <si>
     <t>PC3</t>
   </si>
   <si>
@@ -130,9 +123,6 @@
     <t>03.03.03.03.03</t>
   </si>
   <si>
-    <t>3 chemin des dcd, 75003, Paris</t>
-  </si>
-  <si>
     <t>PC4</t>
   </si>
   <si>
@@ -151,9 +141,6 @@
     <t>04.04.04.04.04</t>
   </si>
   <si>
-    <t>marié</t>
-  </si>
-  <si>
     <t>965 boulevard diablotin, 75006, Paris</t>
   </si>
   <si>
@@ -166,9 +153,6 @@
     <t>PP1</t>
   </si>
   <si>
-    <t>baptiste75001@yopmail.com</t>
-  </si>
-  <si>
     <t>Purain</t>
   </si>
   <si>
@@ -190,9 +174,6 @@
     <t>PP2</t>
   </si>
   <si>
-    <t>jessica.epolas@yopmail.com</t>
-  </si>
-  <si>
     <t>Epolas</t>
   </si>
   <si>
@@ -211,9 +192,6 @@
     <t>PP3</t>
   </si>
   <si>
-    <t>naomie.hun@yopmail.com</t>
-  </si>
-  <si>
     <t>Hun</t>
   </si>
   <si>
@@ -232,9 +210,6 @@
     <t>PP4</t>
   </si>
   <si>
-    <t>christelle.crystal@yopmail.com</t>
-  </si>
-  <si>
     <t>Crystal</t>
   </si>
   <si>
@@ -295,21 +270,12 @@
     <t>SPE1</t>
   </si>
   <si>
-    <t>cardiologie</t>
-  </si>
-  <si>
     <t>SPE2</t>
   </si>
   <si>
-    <t>chamanerie</t>
-  </si>
-  <si>
     <t>SPE3</t>
   </si>
   <si>
-    <t>exorcisme</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -412,15 +378,6 @@
     <t>NS4</t>
   </si>
   <si>
-    <t>Lulu</t>
-  </si>
-  <si>
-    <t>lulu.umul@yopmail.com</t>
-  </si>
-  <si>
-    <t>01.01.01.01.03</t>
-  </si>
-  <si>
     <t>PC5</t>
   </si>
   <si>
@@ -446,17 +403,233 @@
   </si>
   <si>
     <t>Diagnostic 4</t>
+  </si>
+  <si>
+    <t>Laure</t>
+  </si>
+  <si>
+    <t>laure.umul@yopmail.com</t>
+  </si>
+  <si>
+    <t>Aubervilliers</t>
+  </si>
+  <si>
+    <t>06.56.35.94.65</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>louis.fungo@yopmail.com</t>
+  </si>
+  <si>
+    <t>Fungo</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Drancy</t>
+  </si>
+  <si>
+    <t>06.46.26.53.45</t>
+  </si>
+  <si>
+    <t>45 avenue du Tonon, 93100 Montreuil</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>jenifer.freeman@yopmail.com</t>
+  </si>
+  <si>
+    <t>Freeman</t>
+  </si>
+  <si>
+    <t>Jenifer</t>
+  </si>
+  <si>
+    <t>Locambo(Australie)</t>
+  </si>
+  <si>
+    <t>06.54.78.98.95</t>
+  </si>
+  <si>
+    <t>100 rue des arts micheaux, 75019 Paris</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>durand.marie@yopmail.com</t>
+  </si>
+  <si>
+    <t>Durand</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Toulon</t>
+  </si>
+  <si>
+    <t>04.67.46.00.33</t>
+  </si>
+  <si>
+    <t>2 place de la république, 34200 Sète</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>culibri.jessica@yopmail.com</t>
+  </si>
+  <si>
+    <t>Culibri</t>
+  </si>
+  <si>
+    <t>Melun</t>
+  </si>
+  <si>
+    <t>06.27.92.19.48</t>
+  </si>
+  <si>
+    <t>Célibataire</t>
+  </si>
+  <si>
+    <t>23 boulevard Galilée, 93160 Noisy-le-Grand</t>
+  </si>
+  <si>
+    <t>SPE4</t>
+  </si>
+  <si>
+    <t>Chirurgie plastique</t>
+  </si>
+  <si>
+    <t>Dermatologie</t>
+  </si>
+  <si>
+    <t>Gastro-entérologie</t>
+  </si>
+  <si>
+    <t>Gynécologie-obstétrique</t>
+  </si>
+  <si>
+    <t>SPE5</t>
+  </si>
+  <si>
+    <t>Gériatrie</t>
+  </si>
+  <si>
+    <t>Neurologie</t>
+  </si>
+  <si>
+    <t>Ophtalmologie</t>
+  </si>
+  <si>
+    <t>Oncologie</t>
+  </si>
+  <si>
+    <t>Odontologie</t>
+  </si>
+  <si>
+    <t>Oto-rhino-laryngologie</t>
+  </si>
+  <si>
+    <t>Pédiatrie</t>
+  </si>
+  <si>
+    <t>Parodontologie</t>
+  </si>
+  <si>
+    <t>Rhumatologie</t>
+  </si>
+  <si>
+    <t>Radiologie</t>
+  </si>
+  <si>
+    <t>Réanimation médicale</t>
+  </si>
+  <si>
+    <t>Tabacologie</t>
+  </si>
+  <si>
+    <t>SPE6</t>
+  </si>
+  <si>
+    <t>SPE7</t>
+  </si>
+  <si>
+    <t>SPE8</t>
+  </si>
+  <si>
+    <t>SPE9</t>
+  </si>
+  <si>
+    <t>SPE10</t>
+  </si>
+  <si>
+    <t>SPE11</t>
+  </si>
+  <si>
+    <t>SPE12</t>
+  </si>
+  <si>
+    <t>SPE13</t>
+  </si>
+  <si>
+    <t>SPE14</t>
+  </si>
+  <si>
+    <t>SPE15</t>
+  </si>
+  <si>
+    <t>SPE16</t>
+  </si>
+  <si>
+    <t>SPE17</t>
+  </si>
+  <si>
+    <t>Cardiologie</t>
+  </si>
+  <si>
+    <t>Marié</t>
+  </si>
+  <si>
+    <t>Mariée</t>
+  </si>
+  <si>
+    <t>baptiste75001@aphp.com</t>
+  </si>
+  <si>
+    <t>jessica.epolas@aphp.com</t>
+  </si>
+  <si>
+    <t>naomie.hun@aphp.com</t>
+  </si>
+  <si>
+    <t>christelle.crystal@aphp.com</t>
+  </si>
+  <si>
+    <t>10 rue de la roue, 75001, Paris</t>
+  </si>
+  <si>
+    <t>3 chemin des lilas, 75003, Paris</t>
+  </si>
+  <si>
+    <t>20 allée du cimetière, 75002, Paris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -507,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -516,6 +689,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -796,24 +975,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="11" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="31.83203125" customWidth="1"/>
+    <col min="11" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.1" customHeight="1">
+    <row r="2" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -856,7 +1035,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -873,28 +1052,28 @@
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="1">
+        <v>175027511365435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1">
-        <v>1750275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>36556</v>
@@ -903,27 +1082,30 @@
         <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3">
+        <v>100017512039557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F4" s="3">
         <v>38346</v>
@@ -932,101 +1114,263 @@
         <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4">
+        <v>204127511739676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="C5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F5" s="3">
         <v>18943</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="14.1" customHeight="1">
+        <v>33</v>
+      </c>
+      <c r="K5">
+        <v>151111320763138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="2">
+        <v>26171</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="2">
-        <v>27426</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K6" s="1">
+        <v>271089300157430</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1750272</v>
-      </c>
+      <c r="B7" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="10">
+        <v>27226</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K7">
+        <v>174079302968731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="10">
+        <v>26550</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8">
+        <v>272099950141230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="10">
+        <v>14387</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="K9">
+        <v>239058313719460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="10">
+        <v>34233</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K10">
+        <v>293097747038569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="43.42578125" customWidth="1"/>
-    <col min="12" max="1026" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="43.5" customWidth="1"/>
+    <col min="12" max="1026" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1061,30 +1405,30 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G2" s="3">
         <v>29517</v>
@@ -1093,39 +1437,39 @@
         <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2">
         <v>33768</v>
@@ -1134,80 +1478,80 @@
         <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L3" s="1">
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G4" s="2">
         <v>22100</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L4" s="1">
         <v>3</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2">
         <v>32640</v>
@@ -1216,42 +1560,46 @@
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{BBA231E0-6221-4B98-BBDC-9814F6E47C3E}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,108 +1607,108 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1370,48 +1718,160 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+        <v>75</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1421,19 +1881,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,27 +1901,27 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2">
         <v>43476</v>
@@ -1471,18 +1931,18 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2">
         <v>43508</v>
@@ -1492,18 +1952,18 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2">
         <v>43509</v>
@@ -1513,18 +1973,18 @@
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C5" s="2">
         <v>43510</v>
@@ -1534,18 +1994,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2">
         <v>43511</v>
@@ -1555,27 +2015,27 @@
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2">
         <v>43512</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1585,91 +2045,91 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1679,91 +2139,91 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1773,69 +2233,69 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>